<commit_message>
Update Thiết kế giao diện (Danh sách biến cố, danh sách thành phần).xlsx
</commit_message>
<xml_diff>
--- a/Thiết kế/Thiết kế giao diện/Phần thiết kế giao diện (Kim Long)/Thiết kế giao diện (Danh sách biến cố, danh sách thành phần).xlsx
+++ b/Thiết kế/Thiết kế giao diện/Phần thiết kế giao diện (Kim Long)/Thiết kế giao diện (Danh sách biến cố, danh sách thành phần).xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\CNPM\Thiết kế\Thiết kế giao diện\Phần thiết kế giao diện (Kim Long)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\CNPM\Thiết kế\Thiết kế giao diện\Phần thiết kế giao diện (Kim Long)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78139C66-CB5F-4E1F-959A-2E3AD44BF4ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A51CEF-9685-4614-9A5F-5D914DDF2295}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7170" yWindow="1470" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{8DCD9B5B-1C87-4F7B-A019-5F8D8FAA8E49}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{8DCD9B5B-1C87-4F7B-A019-5F8D8FAA8E49}"/>
   </bookViews>
   <sheets>
     <sheet name="Đăng nhập" sheetId="1" r:id="rId1"/>
     <sheet name="Cập nhật đơn hàng" sheetId="2" r:id="rId2"/>
     <sheet name="Cập nhật khách hàng" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
+    <sheet name="Thêm khách hàng" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="123">
   <si>
     <t>Danh sách các biến cố</t>
   </si>
@@ -355,9 +355,6 @@
   </si>
   <si>
     <t>Nhập số điện thoại (chỉ nhập số)</t>
-  </si>
-  <si>
-    <t>Text FIeld</t>
   </si>
   <si>
     <t>abd@gmail.com</t>
@@ -1903,58 +1900,58 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6480E005-811A-4EEC-81E8-0C53857A84FC}" name="Table6" displayName="Table6" ref="A21:D24" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6480E005-811A-4EEC-81E8-0C53857A84FC}" name="Table6" displayName="Table6" ref="A21:D24" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
   <autoFilter ref="A21:D24" xr:uid="{CD914CC4-CC91-422F-B6A4-47838AEBC8F4}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{FE853A7F-07E2-41E6-B2D1-7D56358C9E31}" name="STT" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{B5A3570E-7701-437F-934C-6E1D5532134B}" name="Điều kiện kích hoạt" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{18513E98-EC8D-4FB3-A584-6B682CA9EC5C}" name="Xử lí" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{D324A875-14F9-4BC9-B030-417A8F579A25}" name="Ghi chú" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{FE853A7F-07E2-41E6-B2D1-7D56358C9E31}" name="STT" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{B5A3570E-7701-437F-934C-6E1D5532134B}" name="Điều kiện kích hoạt" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{18513E98-EC8D-4FB3-A584-6B682CA9EC5C}" name="Xử lí" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{D324A875-14F9-4BC9-B030-417A8F579A25}" name="Ghi chú" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{87B3F6DC-585D-4D0A-A114-7051A939A004}" name="Table7" displayName="Table7" ref="A27:G41" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{87B3F6DC-585D-4D0A-A114-7051A939A004}" name="Table7" displayName="Table7" ref="A27:G41" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="A27:G41" xr:uid="{A8BA366D-83A5-449B-9879-6D8A0F0FE1D2}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{F7D873C8-353C-463D-A75C-E918B69801F3}" name="STT" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{84D33AE5-B676-470C-89A4-29C4ADC9E8F9}" name="Tên" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{E84A4A18-6C02-4A70-886E-2314EA3A4237}" name="Kiểu" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{2CBDBD19-F32F-41C1-8BC0-DE7AFF2F8E79}" name="Ý nghĩa" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{BFB1EFA9-6A2D-4AE1-AFC7-9FA5E34E33FA}" name="Miền giá trị " dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{2C4B2AC0-AD02-4B2B-8CDE-DD216FB98B24}" name="Giá trị mặc định" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{B1E4F1B8-3E2F-4101-9A1C-5DAE809CB153}" name="Ghi chú" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{F7D873C8-353C-463D-A75C-E918B69801F3}" name="STT" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{84D33AE5-B676-470C-89A4-29C4ADC9E8F9}" name="Tên" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{E84A4A18-6C02-4A70-886E-2314EA3A4237}" name="Kiểu" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{2CBDBD19-F32F-41C1-8BC0-DE7AFF2F8E79}" name="Ý nghĩa" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{BFB1EFA9-6A2D-4AE1-AFC7-9FA5E34E33FA}" name="Miền giá trị " dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{2C4B2AC0-AD02-4B2B-8CDE-DD216FB98B24}" name="Giá trị mặc định" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{B1E4F1B8-3E2F-4101-9A1C-5DAE809CB153}" name="Ghi chú" dataDxfId="15"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{10DF9716-C5EF-40F6-A78C-32A3FF7718F9}" name="Table8" displayName="Table8" ref="A26:D29" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{10DF9716-C5EF-40F6-A78C-32A3FF7718F9}" name="Table8" displayName="Table8" ref="A26:D29" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="A26:D29" xr:uid="{D90D3593-5FE2-4DE1-8A0D-DD996F585FA2}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{51834C17-D72E-4F06-A8AA-121CCD274B90}" name="STT" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{16A3EAFB-8894-4CDB-8E69-BA6873647141}" name="Điều kiện kích hoạt" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{0E4333BA-17BF-41F8-8058-D206BEC44F14}" name="Xử lí" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{9C83F13B-2CC2-4ADB-8EDE-8887EDFDDEAF}" name="Ghi chú" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{51834C17-D72E-4F06-A8AA-121CCD274B90}" name="STT" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{16A3EAFB-8894-4CDB-8E69-BA6873647141}" name="Điều kiện kích hoạt" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{0E4333BA-17BF-41F8-8058-D206BEC44F14}" name="Xử lí" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{9C83F13B-2CC2-4ADB-8EDE-8887EDFDDEAF}" name="Ghi chú" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F5270894-4E51-450C-9A6D-02B4DD40513A}" name="Table1" displayName="Table1" ref="A32:G46" totalsRowShown="0" headerRowDxfId="15" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F5270894-4E51-450C-9A6D-02B4DD40513A}" name="Table1" displayName="Table1" ref="A32:G46" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A32:G46" xr:uid="{120F98EB-2A33-4BA0-8718-FCFED55F678F}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{C2074B14-666B-4C0A-BB88-DEF0B9EE0D43}" name="STT" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{29476051-443B-4A4D-AE15-F4801782B1A1}" name="Tên" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{BCE422A5-BAA1-42EA-8858-57BE75951A80}" name="Kiểu" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{1F566541-47B3-4A3B-A7EC-C79E5E756808}" name="Ý nghĩa" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{5EA9C6D3-DB97-452C-9BA5-28CD21962BE1}" name="Miền giá trị" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{419FD13A-0101-44D6-B26D-BABEEB84B949}" name="Giá trị mặc định" dataDxfId="18"/>
-    <tableColumn id="7" xr3:uid="{236F72AC-545A-4EE3-A793-09FC7687AE23}" name="Ghi chú" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{C2074B14-666B-4C0A-BB88-DEF0B9EE0D43}" name="STT" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{29476051-443B-4A4D-AE15-F4801782B1A1}" name="Tên" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{BCE422A5-BAA1-42EA-8858-57BE75951A80}" name="Kiểu" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{1F566541-47B3-4A3B-A7EC-C79E5E756808}" name="Ý nghĩa" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{5EA9C6D3-DB97-452C-9BA5-28CD21962BE1}" name="Miền giá trị" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{419FD13A-0101-44D6-B26D-BABEEB84B949}" name="Giá trị mặc định" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{236F72AC-545A-4EE3-A793-09FC7687AE23}" name="Ghi chú" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2259,7 +2256,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D58451-CBD0-4663-8FD9-73FB008247F8}">
   <dimension ref="A14:G28"/>
   <sheetViews>
-    <sheetView topLeftCell="A119" zoomScale="80" workbookViewId="0">
+    <sheetView zoomScale="80" workbookViewId="0">
       <selection activeCell="A129" sqref="A129:G150"/>
     </sheetView>
   </sheetViews>
@@ -2846,7 +2843,7 @@
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
     </row>
-    <row r="52" spans="1:7" ht="58.5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" ht="39" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>8</v>
       </c>
@@ -2857,7 +2854,7 @@
         <v>60</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
@@ -2877,7 +2874,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60902CDE-C5A7-43A1-BB39-B9206B721EBF}">
   <dimension ref="A20:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D27" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
@@ -3080,13 +3077,13 @@
         <v>8</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -3094,13 +3091,13 @@
         <v>9</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -3108,13 +3105,13 @@
         <v>10</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -3122,13 +3119,13 @@
         <v>11</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -3136,13 +3133,13 @@
         <v>12</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -3150,13 +3147,13 @@
         <v>13</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
@@ -3164,13 +3161,13 @@
         <v>14</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -3191,8 +3188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B53652B8-F3FD-489D-80A8-13F24383F997}">
   <dimension ref="A25:G46"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3421,7 +3418,7 @@
         <v>93</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>107</v>
+        <v>66</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>94</v>
@@ -3446,7 +3443,7 @@
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="19.5" x14ac:dyDescent="0.3">
@@ -3454,13 +3451,13 @@
         <v>8</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -3471,13 +3468,13 @@
         <v>9</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
@@ -3488,13 +3485,13 @@
         <v>10</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
@@ -3505,13 +3502,13 @@
         <v>11</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
@@ -3522,13 +3519,13 @@
         <v>12</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -3539,13 +3536,13 @@
         <v>13</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
@@ -3556,13 +3553,13 @@
         <v>14</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>

</xml_diff>